<commit_message>
changes to param file and solver -100 to 100
</commit_message>
<xml_diff>
--- a/python_single_shooting/parameters.xlsx
+++ b/python_single_shooting/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karls\Dirac\ShootingDirac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\Shooting_Dirac\python_single_shooting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD3B276-5BB6-4C90-A39C-4926711B4E20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC6A1D7-D329-4C09-AB14-20F384CFCB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13950" yWindow="4575" windowWidth="33330" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +587,12 @@
       <c r="H4">
         <v>3.2429999999999998E-3</v>
       </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>